<commit_message>
aligned states at different angles, fixing error ran test run of l_assignment
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_3_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_3_spec_factors.xlsx
@@ -383,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E1"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,6 +401,1060 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2183</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.04521315146650687</v>
+      </c>
+      <c r="E2">
+        <v>0.0007548780721989336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2205</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.01611679227055696</v>
+      </c>
+      <c r="E3">
+        <v>0.0004348996575589752</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2232</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.03518987793411343</v>
+      </c>
+      <c r="E4">
+        <v>0.0006351030734999646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2542.566758096668</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.01348835594041631</v>
+      </c>
+      <c r="E5">
+        <v>0.001582817278722323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2552.302019868146</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.01734939901769974</v>
+      </c>
+      <c r="E6">
+        <v>0.001474356043006104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2564.932497649873</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.02109502145306891</v>
+      </c>
+      <c r="E7">
+        <v>0.001399507895753763</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2576.595223088505</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.02114515460690668</v>
+      </c>
+      <c r="E8">
+        <v>0.001325821591108297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2604.774782462973</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.01488134806343017</v>
+      </c>
+      <c r="E9">
+        <v>0.00151506937297366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2619.805711625691</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.03062457611001244</v>
+      </c>
+      <c r="E10">
+        <v>0.00184485398253087</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2633.047356124614</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.004271137648865483</v>
+      </c>
+      <c r="E11">
+        <v>0.001101152675098133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2641.986500425834</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.0127502231274668</v>
+      </c>
+      <c r="E12">
+        <v>0.00116516399337164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2656.691278730293</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.01606539268759116</v>
+      </c>
+      <c r="E13">
+        <v>0.001225607277197675</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2671.645712477859</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.006828096843831242</v>
+      </c>
+      <c r="E14">
+        <v>0.0009895792527291653</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2700.381836639923</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.01798880889865299</v>
+      </c>
+      <c r="E15">
+        <v>0.001305902642370454</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2713.252982858696</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.02740469432961291</v>
+      </c>
+      <c r="E16">
+        <v>0.001464621430917555</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>2726.840802344541</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.0106275175474632</v>
+      </c>
+      <c r="E17">
+        <v>0.0009396280758427827</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>2746.363762576609</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0.02832420701350039</v>
+      </c>
+      <c r="E18">
+        <v>0.001770262938343775</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>2758.880085527932</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.01604327730689366</v>
+      </c>
+      <c r="E19">
+        <v>0.001668500839916941</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>2777.181176406648</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0.02758892405816186</v>
+      </c>
+      <c r="E20">
+        <v>0.002267145379779505</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>2787</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0.05482263607755739</v>
+      </c>
+      <c r="E21">
+        <v>0.002416775140309955</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>2827.101259227846</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.008703231009402439</v>
+      </c>
+      <c r="E22">
+        <v>0.0008169097698356079</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>2841.959721907576</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.002595176403055325</v>
+      </c>
+      <c r="E23">
+        <v>0.0006253437115795967</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>2869.514732511383</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.01820856044503889</v>
+      </c>
+      <c r="E24">
+        <v>0.0009926302116545903</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>2887.503509710963</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.01505668650932555</v>
+      </c>
+      <c r="E25">
+        <v>0.003239655908768817</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>2894.579211705925</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0.01400753463110854</v>
+      </c>
+      <c r="E26">
+        <v>0.003047793249406033</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>2907.129675101117</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0.01012029601546606</v>
+      </c>
+      <c r="E27">
+        <v>0.001073364728913067</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>2924.234342911454</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0.008616412004231768</v>
+      </c>
+      <c r="E28">
+        <v>0.0009166395749182732</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>2936.124980912122</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0.0231391268409352</v>
+      </c>
+      <c r="E29">
+        <v>0.001096063902991668</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>2959.117122042539</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0.0281805909964225</v>
+      </c>
+      <c r="E30">
+        <v>0.001148994053502205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>2982.864196645418</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0.005284657897110587</v>
+      </c>
+      <c r="E31">
+        <v>0.0007506616331122993</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>2998.883965523738</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0.01563948893783618</v>
+      </c>
+      <c r="E32">
+        <v>0.001704494970280426</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>3007.118657087334</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0.0163814842057683</v>
+      </c>
+      <c r="E33">
+        <v>0.001760487373661803</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>3064</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0.01351368052201604</v>
+      </c>
+      <c r="E34">
+        <v>0.0005782599091517874</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>3081.813926466619</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0.004723229169723403</v>
+      </c>
+      <c r="E35">
+        <v>0.000434083879845237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>3096.712914411186</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.006935106148217499</v>
+      </c>
+      <c r="E36">
+        <v>0.0003948031856736916</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>3133.618862442509</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0.003896092063913702</v>
+      </c>
+      <c r="E37">
+        <v>0.0003035599781892204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>3155.20165968082</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0.002353854634804682</v>
+      </c>
+      <c r="E38">
+        <v>0.0004032609371447396</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>3168.125784376794</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0.004587456023074017</v>
+      </c>
+      <c r="E39">
+        <v>0.0006450762403180628</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>3180.855405406395</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0.009002520224109845</v>
+      </c>
+      <c r="E40">
+        <v>0.0006794869555669696</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>3192.810075633211</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0.007799363770547631</v>
+      </c>
+      <c r="E41">
+        <v>0.0005225779646063982</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>3224.072026396334</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0.003426628027337729</v>
+      </c>
+      <c r="E42">
+        <v>0.000399207048345339</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>3243.873355870091</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0.002567171024052742</v>
+      </c>
+      <c r="E43">
+        <v>0.0003266239702657703</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>3259.461277156505</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.00415570834958121</v>
+      </c>
+      <c r="E44">
+        <v>0.0003868464931322279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>3275.706563811741</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.005197445182185524</v>
+      </c>
+      <c r="E45">
+        <v>0.0003691095623350285</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>3297.170677130526</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0.01233122541749084</v>
+      </c>
+      <c r="E46">
+        <v>0.0008571031119780627</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>3322.739257221813</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0.002806152843716178</v>
+      </c>
+      <c r="E47">
+        <v>0.000550226047787486</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>3340.274605893867</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0.007122075727266107</v>
+      </c>
+      <c r="E48">
+        <v>0.0006848149737755874</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>3363.00085761773</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0.009646823953053706</v>
+      </c>
+      <c r="E49">
+        <v>0.0008720292838918605</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>3380.649591047521</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0.01082571747791658</v>
+      </c>
+      <c r="E50">
+        <v>0.0009767564641729243</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>3395.65849793409</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0.006650910660026634</v>
+      </c>
+      <c r="E51">
+        <v>0.0008651591102473671</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>3411.582461109694</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0.01223640478000984</v>
+      </c>
+      <c r="E52">
+        <v>0.0008355254365204956</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>3430.405841076768</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0.007624066039287261</v>
+      </c>
+      <c r="E53">
+        <v>0.0006979778768361577</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>3452.040838634491</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0.009753580600208962</v>
+      </c>
+      <c r="E54">
+        <v>0.0007482198816598655</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>3477.521886486277</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0.005594811456957265</v>
+      </c>
+      <c r="E55">
+        <v>0.001758369315043712</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>3485.00198550665</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0.006611789611757523</v>
+      </c>
+      <c r="E56">
+        <v>0.001433882084477535</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>3503.741363695906</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0.01904078020967842</v>
+      </c>
+      <c r="E57">
+        <v>0.001560286156070871</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>3521.461101658533</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0.006458707341395495</v>
+      </c>
+      <c r="E58">
+        <v>0.001397189751403923</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>3536.043535477974</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0.00275976649513679</v>
+      </c>
+      <c r="E59">
+        <v>0.0006570872607468547</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>3545.218978961481</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0.01826155602808355</v>
+      </c>
+      <c r="E60">
+        <v>0.001233179789252768</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>3561.667933967139</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0.007296542395219974</v>
+      </c>
+      <c r="E61">
+        <v>0.0009414893413187063</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>3580.019183465469</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0.006267172453982193</v>
+      </c>
+      <c r="E62">
+        <v>0.0009923023052138471</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>3589.932337372161</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0.01898071528820476</v>
+      </c>
+      <c r="E63">
+        <v>0.0009633559199774704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
got distributions for bite 3 modified run properties to change the cross sections
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_3_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_3_spec_factors.xlsx
@@ -414,10 +414,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.04521315146650687</v>
+        <v>0.1003833467679155</v>
       </c>
       <c r="E2">
-        <v>0.0007548780721989336</v>
+        <v>0.002633670046383253</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -428,13 +428,13 @@
         <v>2205</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0.01611679227055696</v>
+        <v>0.01967941761905094</v>
       </c>
       <c r="E3">
-        <v>0.0004348996575589752</v>
+        <v>0.001346880293319076</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -445,13 +445,13 @@
         <v>2232</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.03518987793411343</v>
+        <v>0.05943802801823975</v>
       </c>
       <c r="E4">
-        <v>0.0006351030734999646</v>
+        <v>0.001053883381133756</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -462,13 +462,13 @@
         <v>2542.566758096668</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>0.01348835594041631</v>
+        <v>0.01003317029389575</v>
       </c>
       <c r="E5">
-        <v>0.001582817278722323</v>
+        <v>0.001693911867800581</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -476,16 +476,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2552.302019868146</v>
+        <v>2552.302019868145</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0.01734939901769974</v>
+        <v>0.01383371637882464</v>
       </c>
       <c r="E6">
-        <v>0.001474356043006104</v>
+        <v>0.0007008793442481233</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -496,13 +496,13 @@
         <v>2564.932497649873</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>0.02109502145306891</v>
+        <v>0.01187085410814768</v>
       </c>
       <c r="E7">
-        <v>0.001399507895753763</v>
+        <v>0.001427097215187148</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -510,16 +510,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2576.595223088505</v>
+        <v>2576.595223088504</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0.02114515460690668</v>
+        <v>0.01749281742997389</v>
       </c>
       <c r="E8">
-        <v>0.001325821591108297</v>
+        <v>0.000670410960262062</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -530,13 +530,13 @@
         <v>2604.774782462973</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>0.01488134806343017</v>
+        <v>0.008630323237560395</v>
       </c>
       <c r="E9">
-        <v>0.00151506937297366</v>
+        <v>0.00112858073106559</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -547,13 +547,13 @@
         <v>2619.805711625691</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0.03062457611001244</v>
+        <v>0.02695315010985294</v>
       </c>
       <c r="E10">
-        <v>0.00184485398253087</v>
+        <v>0.001059372864211382</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -564,13 +564,13 @@
         <v>2633.047356124614</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0.004271137648865483</v>
+        <v>0.003118765279171087</v>
       </c>
       <c r="E11">
-        <v>0.001101152675098133</v>
+        <v>0.0006307310414617373</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -581,13 +581,13 @@
         <v>2641.986500425834</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>0.0127502231274668</v>
+        <v>0.01153263396511821</v>
       </c>
       <c r="E12">
-        <v>0.00116516399337164</v>
+        <v>0.0006702065028555223</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -598,13 +598,13 @@
         <v>2656.691278730293</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>0.01606539268759116</v>
+        <v>0.01477815843567994</v>
       </c>
       <c r="E13">
-        <v>0.001225607277197675</v>
+        <v>0.0007604345812864912</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -615,13 +615,13 @@
         <v>2671.645712477859</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.006828096843831242</v>
+        <v>0.007289291180016085</v>
       </c>
       <c r="E14">
-        <v>0.0009895792527291653</v>
+        <v>0.0006598198330066742</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -632,13 +632,13 @@
         <v>2700.381836639923</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.01798880889865299</v>
+        <v>0.01800662804138555</v>
       </c>
       <c r="E15">
-        <v>0.001305902642370454</v>
+        <v>0.000931406133057303</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -649,13 +649,13 @@
         <v>2713.252982858696</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>0.02740469432961291</v>
+        <v>0.01534716269474826</v>
       </c>
       <c r="E16">
-        <v>0.001464621430917555</v>
+        <v>0.0006263605004839691</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -666,13 +666,13 @@
         <v>2726.840802344541</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0.0106275175474632</v>
+        <v>0.0104679443723541</v>
       </c>
       <c r="E17">
-        <v>0.0009396280758427827</v>
+        <v>0.0005962120273638413</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -683,13 +683,13 @@
         <v>2746.363762576609</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0.02832420701350039</v>
+        <v>0.0278026913402598</v>
       </c>
       <c r="E18">
-        <v>0.001770262938343775</v>
+        <v>0.001103103675507483</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -700,13 +700,13 @@
         <v>2758.880085527932</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0.01604327730689366</v>
+        <v>0.01406444463080108</v>
       </c>
       <c r="E19">
-        <v>0.001668500839916941</v>
+        <v>0.001024149975157255</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -717,13 +717,13 @@
         <v>2777.181176406648</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>0.02758892405816186</v>
+        <v>0.01644381189109301</v>
       </c>
       <c r="E20">
-        <v>0.002267145379779505</v>
+        <v>0.001688147988819468</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -734,13 +734,13 @@
         <v>2787</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0.05482263607755739</v>
+        <v>0.04967761623345822</v>
       </c>
       <c r="E21">
-        <v>0.002416775140309955</v>
+        <v>0.001238525999353802</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -751,13 +751,13 @@
         <v>2827.101259227846</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>0.008703231009402439</v>
+        <v>0.004770638388218259</v>
       </c>
       <c r="E22">
-        <v>0.0008169097698356079</v>
+        <v>0.0008673887978578587</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -768,13 +768,13 @@
         <v>2841.959721907576</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>0.002595176403055325</v>
+        <v>0.001173930436090106</v>
       </c>
       <c r="E23">
-        <v>0.0006253437115795967</v>
+        <v>0.0006796439366837606</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -785,13 +785,13 @@
         <v>2869.514732511383</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0.01820856044503889</v>
+        <v>0.01786830746375652</v>
       </c>
       <c r="E24">
-        <v>0.0009926302116545903</v>
+        <v>0.0006846600141425562</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -802,13 +802,13 @@
         <v>2887.503509710963</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0.01505668650932555</v>
+        <v>0.01872632096582117</v>
       </c>
       <c r="E25">
-        <v>0.003239655908768817</v>
+        <v>0.001673442769643433</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -822,10 +822,10 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>0.01400753463110854</v>
+        <v>0.0147537232516338</v>
       </c>
       <c r="E26">
-        <v>0.003047793249406033</v>
+        <v>0.003902252889019084</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -836,13 +836,13 @@
         <v>2907.129675101117</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>0.01012029601546606</v>
+        <v>0.006905271629601476</v>
       </c>
       <c r="E27">
-        <v>0.001073364728913067</v>
+        <v>0.001038846174364854</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -856,10 +856,10 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0.008616412004231768</v>
+        <v>0.006815869725090891</v>
       </c>
       <c r="E28">
-        <v>0.0009166395749182732</v>
+        <v>0.002039394090972078</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -873,10 +873,10 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>0.0231391268409352</v>
+        <v>0.03107694530033408</v>
       </c>
       <c r="E29">
-        <v>0.001096063902991668</v>
+        <v>0.00204312097130224</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -890,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0.0281805909964225</v>
+        <v>0.04964234777733157</v>
       </c>
       <c r="E30">
-        <v>0.001148994053502205</v>
+        <v>0.001996485725827465</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -904,13 +904,13 @@
         <v>2982.864196645418</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D31">
-        <v>0.005284657897110587</v>
+        <v>0.007916632780802336</v>
       </c>
       <c r="E31">
-        <v>0.0007506616331122993</v>
+        <v>0.0008633424786485272</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -924,10 +924,10 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0.01563948893783618</v>
+        <v>0.0159103685394359</v>
       </c>
       <c r="E32">
-        <v>0.001704494970280426</v>
+        <v>0.002823683153756541</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -938,13 +938,13 @@
         <v>3007.118657087334</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>0.0163814842057683</v>
+        <v>0.01788892509131872</v>
       </c>
       <c r="E33">
-        <v>0.001760487373661803</v>
+        <v>0.001245416013572331</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -958,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>0.01351368052201604</v>
+        <v>0.03463617967285389</v>
       </c>
       <c r="E34">
-        <v>0.0005782599091517874</v>
+        <v>0.002913837337557551</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -975,10 +975,10 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>0.004723229169723403</v>
+        <v>0.01025786663621027</v>
       </c>
       <c r="E35">
-        <v>0.000434083879845237</v>
+        <v>0.001599344798118806</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -989,13 +989,13 @@
         <v>3096.712914411186</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>0.006935106148217499</v>
+        <v>0.007476346500770412</v>
       </c>
       <c r="E36">
-        <v>0.0003948031856736916</v>
+        <v>0.001027284252014255</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1009,10 +1009,10 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>0.003896092063913702</v>
+        <v>0.01237648045970882</v>
       </c>
       <c r="E37">
-        <v>0.0003035599781892204</v>
+        <v>0.00161674744743944</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1026,10 +1026,10 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>0.002353854634804682</v>
+        <v>0.003973759564147854</v>
       </c>
       <c r="E38">
-        <v>0.0004032609371447396</v>
+        <v>0.002406643116314897</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1040,13 +1040,13 @@
         <v>3168.125784376794</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>0.004587456023074017</v>
+        <v>0.00385444869379247</v>
       </c>
       <c r="E39">
-        <v>0.0006450762403180628</v>
+        <v>0.0009496467796300289</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1057,13 +1057,13 @@
         <v>3180.855405406395</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>0.009002520224109845</v>
+        <v>0.008892275482153213</v>
       </c>
       <c r="E40">
-        <v>0.0006794869555669696</v>
+        <v>0.000994530810504012</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1077,10 +1077,10 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>0.007799363770547631</v>
+        <v>0.02308051077533096</v>
       </c>
       <c r="E41">
-        <v>0.0005225779646063982</v>
+        <v>0.002778734712509133</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1091,13 +1091,13 @@
         <v>3224.072026396334</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>0.003426628027337729</v>
+        <v>0.003778260321143645</v>
       </c>
       <c r="E42">
-        <v>0.000399207048345339</v>
+        <v>0.001104414555411244</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1108,13 +1108,13 @@
         <v>3243.873355870091</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D43">
-        <v>0.002567171024052742</v>
+        <v>0.002493016360014469</v>
       </c>
       <c r="E43">
-        <v>0.0003266239702657703</v>
+        <v>0.0002627792643487508</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1122,16 +1122,16 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>3259.461277156505</v>
+        <v>3259.461277156506</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>0.00415570834958121</v>
+        <v>0.003520979003111298</v>
       </c>
       <c r="E44">
-        <v>0.0003868464931322279</v>
+        <v>0.001029209247063302</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1142,13 +1142,13 @@
         <v>3275.706563811741</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>0.005197445182185524</v>
+        <v>0.006690400924903099</v>
       </c>
       <c r="E45">
-        <v>0.0003691095623350285</v>
+        <v>0.0004779330702489417</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1159,13 +1159,13 @@
         <v>3297.170677130526</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>0.01233122541749084</v>
+        <v>0.007114685598151072</v>
       </c>
       <c r="E46">
-        <v>0.0008571031119780627</v>
+        <v>0.0008559020268452416</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1173,16 +1173,16 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>3322.739257221813</v>
+        <v>3322.739257221812</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>0.002806152843716178</v>
+        <v>0.004031759145448133</v>
       </c>
       <c r="E47">
-        <v>0.000550226047787486</v>
+        <v>0.000309780126409277</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1193,13 +1193,13 @@
         <v>3340.274605893867</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
-        <v>0.007122075727266107</v>
+        <v>0.008720165543479061</v>
       </c>
       <c r="E48">
-        <v>0.0006848149737755874</v>
+        <v>0.000382519680734768</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1210,13 +1210,13 @@
         <v>3363.00085761773</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>0.009646823953053706</v>
+        <v>0.01098980593122331</v>
       </c>
       <c r="E49">
-        <v>0.0008720292838918605</v>
+        <v>0.000464825000048043</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1227,13 +1227,13 @@
         <v>3380.649591047521</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D50">
-        <v>0.01082571747791658</v>
+        <v>0.007028112719978081</v>
       </c>
       <c r="E50">
-        <v>0.0009767564641729243</v>
+        <v>0.001509742732439736</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1244,13 +1244,13 @@
         <v>3395.65849793409</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>0.006650910660026634</v>
+        <v>0.006788603562007698</v>
       </c>
       <c r="E51">
-        <v>0.0008651591102473671</v>
+        <v>0.0005157876535650174</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1261,13 +1261,13 @@
         <v>3411.582461109694</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <v>0.01223640478000984</v>
+        <v>0.01316921060467234</v>
       </c>
       <c r="E52">
-        <v>0.0008355254365204956</v>
+        <v>0.0004666798297619102</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1278,13 +1278,13 @@
         <v>3430.405841076768</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <v>0.007624066039287261</v>
+        <v>0.008655787788784879</v>
       </c>
       <c r="E53">
-        <v>0.0006979778768361577</v>
+        <v>0.0003797168811668873</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1295,13 +1295,13 @@
         <v>3452.040838634491</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D54">
-        <v>0.009753580600208962</v>
+        <v>0.006101726008472538</v>
       </c>
       <c r="E54">
-        <v>0.0007482198816598655</v>
+        <v>0.0009152589012708806</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1315,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>0.005594811456957265</v>
+        <v>0.006343840521350375</v>
       </c>
       <c r="E55">
-        <v>0.001758369315043712</v>
+        <v>0.001585960130337594</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1326,16 +1326,16 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>3485.00198550665</v>
+        <v>3485.001985506649</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D56">
-        <v>0.006611789611757523</v>
+        <v>0.006843909527091864</v>
       </c>
       <c r="E56">
-        <v>0.001433882084477535</v>
+        <v>0.0009058115550562761</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1346,13 +1346,13 @@
         <v>3503.741363695906</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D57">
-        <v>0.01904078020967842</v>
+        <v>0.01364478371902552</v>
       </c>
       <c r="E57">
-        <v>0.001560286156070871</v>
+        <v>0.001049598747617347</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1363,13 +1363,13 @@
         <v>3521.461101658533</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <v>0.006458707341395495</v>
+        <v>0.005134959864739125</v>
       </c>
       <c r="E58">
-        <v>0.001397189751403923</v>
+        <v>0.0006544222277116336</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1377,16 +1377,16 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>3536.043535477974</v>
+        <v>3536.043535477975</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>0.00275976649513679</v>
+        <v>0.00612602588370704</v>
       </c>
       <c r="E59">
-        <v>0.0006570872607468547</v>
+        <v>0.00637606775651141</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1400,10 +1400,10 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>0.01826155602808355</v>
+        <v>0.04215767530712843</v>
       </c>
       <c r="E60">
-        <v>0.001233179789252768</v>
+        <v>0.00664987140261252</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1414,13 +1414,13 @@
         <v>3561.667933967139</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D61">
-        <v>0.007296542395219974</v>
+        <v>0.007645409937961853</v>
       </c>
       <c r="E61">
-        <v>0.0009414893413187063</v>
+        <v>0.001078198837404877</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1431,13 +1431,13 @@
         <v>3580.019183465469</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D62">
-        <v>0.006267172453982193</v>
+        <v>0.008299175502610256</v>
       </c>
       <c r="E62">
-        <v>0.0009923023052138471</v>
+        <v>0.0006840855412917909</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1451,10 +1451,10 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>0.01898071528820476</v>
+        <v>0.03162934850620898</v>
       </c>
       <c r="E63">
-        <v>0.0009633559199774704</v>
+        <v>0.002231909672817166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added function in l_assignment to remove one angle from the normalisation fixed the 25 degree data made plots with dodgy 25 degree data
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_3_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_3_spec_factors.xlsx
@@ -414,10 +414,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.1003833467679155</v>
+        <v>0.0960744875850935</v>
       </c>
       <c r="E2">
-        <v>0.002633670046383253</v>
+        <v>0.002520622277711838</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -428,13 +428,13 @@
         <v>2205</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0.01967941761905094</v>
+        <v>0.02911706285278049</v>
       </c>
       <c r="E3">
-        <v>0.001346880293319076</v>
+        <v>0.0007742253544701382</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -445,13 +445,13 @@
         <v>2232</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>0.05943802801823975</v>
+        <v>0.08259227143154145</v>
       </c>
       <c r="E4">
-        <v>0.001053883381133756</v>
+        <v>0.001848109445836572</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -459,16 +459,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2542.566758096668</v>
+        <v>2470.366758096668</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0.01003317029389575</v>
+        <v>0.008296784368939976</v>
       </c>
       <c r="E5">
-        <v>0.001693911867800581</v>
+        <v>0.000504062765808345</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -476,16 +476,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2552.302019868145</v>
+        <v>2481.984729487203</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.01383371637882464</v>
+        <v>0.01369947817056663</v>
       </c>
       <c r="E6">
-        <v>0.0007008793442481233</v>
+        <v>0.000694477856152875</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -493,16 +493,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2564.932497649873</v>
+        <v>2497.913976174627</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>0.01187085410814768</v>
+        <v>0.003373297067722395</v>
       </c>
       <c r="E7">
-        <v>0.001427097215187148</v>
+        <v>0.0008187614242044651</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -510,16 +510,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2576.595223088504</v>
+        <v>2569.303537215177</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.01749281742997389</v>
+        <v>0.01728622194449643</v>
       </c>
       <c r="E8">
-        <v>0.000670410960262062</v>
+        <v>0.0006630908488656306</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -527,16 +527,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2604.774782462973</v>
+        <v>2593.831325411606</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>0.008630323237560395</v>
+        <v>0.02208428679384985</v>
       </c>
       <c r="E9">
-        <v>0.00112858073106559</v>
+        <v>0.001495566083159258</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -544,16 +544,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2619.805711625691</v>
+        <v>2609.227572242163</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0.02695315010985294</v>
+        <v>0.0268483955912421</v>
       </c>
       <c r="E10">
-        <v>0.001059372864211382</v>
+        <v>0.001054856487612694</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -561,16 +561,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2633.047356124614</v>
+        <v>2621.783451658836</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0.003118765279171087</v>
+        <v>0.00309447226499785</v>
       </c>
       <c r="E11">
-        <v>0.0006307310414617373</v>
+        <v>0.0006268501198112199</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -578,16 +578,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>2641.986500425834</v>
+        <v>2635.089616413751</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0.01153263396511821</v>
+        <v>0.01149130537220409</v>
       </c>
       <c r="E12">
-        <v>0.0006702065028555223</v>
+        <v>0.0006675264545959958</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -595,16 +595,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>2656.691278730293</v>
+        <v>2649.075587546623</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0.01477815843567994</v>
+        <v>0.01472230434964875</v>
       </c>
       <c r="E13">
-        <v>0.0007604345812864912</v>
+        <v>0.0007573561146787284</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -612,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2671.645712477859</v>
+        <v>2664.601302816965</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -629,7 +629,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2700.381836639923</v>
+        <v>2688.339468084317</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -646,16 +646,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>2713.252982858696</v>
+        <v>2702.26533490114</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>0.01534716269474826</v>
+        <v>0.004391319269637482</v>
       </c>
       <c r="E16">
-        <v>0.0006263605004839691</v>
+        <v>0.0007582133990740976</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -663,7 +663,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>2726.840802344541</v>
+        <v>2715.640802344541</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -680,16 +680,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>2746.363762576609</v>
+        <v>2737.363762576609</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>0.0278026913402598</v>
+        <v>0.02780269134025979</v>
       </c>
       <c r="E18">
-        <v>0.001103103675507483</v>
+        <v>0.00110310367550748</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -697,7 +697,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2758.880085527932</v>
+        <v>2749.680085527932</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -714,16 +714,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>2777.181176406648</v>
+        <v>2767.781176406648</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20">
-        <v>0.01644381189109301</v>
+        <v>0.01853865151391864</v>
       </c>
       <c r="E20">
-        <v>0.001688147988819468</v>
+        <v>0.0005810482725139638</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -731,16 +731,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>2787</v>
+        <v>2779.2</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0.04967761623345822</v>
+        <v>0.07348957557846092</v>
       </c>
       <c r="E21">
-        <v>0.001238525999353802</v>
+        <v>0.002774143209893858</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -748,16 +748,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>2827.101259227846</v>
+        <v>2813.501259227846</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>0.004770638388218259</v>
+        <v>0.003602772433087223</v>
       </c>
       <c r="E22">
-        <v>0.0008673887978578587</v>
+        <v>0.0002126147707377977</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -765,16 +765,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>2841.959721907576</v>
+        <v>2828.359721907576</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.001173930436090106</v>
+        <v>0.002374588601064437</v>
       </c>
       <c r="E23">
-        <v>0.0006796439366837606</v>
+        <v>0.000315379793147412</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -782,16 +782,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2869.514732511383</v>
+        <v>2853.114732511383</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>0.01786830746375652</v>
+        <v>0.01742527498144794</v>
       </c>
       <c r="E24">
-        <v>0.0006846600141425562</v>
+        <v>0.0006691873879849242</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -799,16 +799,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2887.503509710963</v>
+        <v>2875.303509710963</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>0.01872632096582117</v>
+        <v>0.01832457211464001</v>
       </c>
       <c r="E25">
-        <v>0.001673442769643433</v>
+        <v>0.001638985953500033</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -816,16 +816,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>2894.579211705925</v>
+        <v>2884.179211705924</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>0.0147537232516338</v>
+        <v>0.01412043378719112</v>
       </c>
       <c r="E26">
-        <v>0.003902252889019084</v>
+        <v>0.003734752414728085</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -833,16 +833,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2907.129675101117</v>
+        <v>2899.529675101117</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0.006905271629601476</v>
+        <v>0.0189174637352376</v>
       </c>
       <c r="E27">
-        <v>0.001038846174364854</v>
+        <v>0.002153207254417288</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -850,16 +850,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2924.234342911454</v>
+        <v>2917.634342911454</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0.006815869725090891</v>
+        <v>0.006523305033840098</v>
       </c>
       <c r="E28">
-        <v>0.002039394090972078</v>
+        <v>0.001951855049495462</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -867,16 +867,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>2936.124980912122</v>
+        <v>2928.524980912122</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>0.03107694530033408</v>
+        <v>0.02974299713619296</v>
       </c>
       <c r="E29">
-        <v>0.00204312097130224</v>
+        <v>0.001955421957050748</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -884,16 +884,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>2959.117122042539</v>
+        <v>2949.317122042539</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0.04964234777733157</v>
+        <v>0.04751149746237109</v>
       </c>
       <c r="E30">
-        <v>0.001996485725827465</v>
+        <v>0.001910788484899707</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -901,16 +901,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>2982.864196645418</v>
+        <v>2970.664196645418</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31">
-        <v>0.007916632780802336</v>
+        <v>0.006987003767356034</v>
       </c>
       <c r="E31">
-        <v>0.0008633424786485272</v>
+        <v>0.0009924721260448912</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -918,16 +918,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>2998.883965523738</v>
+        <v>2986.283965523739</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0.0159103685394359</v>
+        <v>0.01522743118189063</v>
       </c>
       <c r="E32">
-        <v>0.002823683153756541</v>
+        <v>0.002702479254123934</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -935,16 +935,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>3007.118657087334</v>
+        <v>2997.718657087334</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>0.01788892509131872</v>
+        <v>0.01747133954907086</v>
       </c>
       <c r="E33">
-        <v>0.001245416013572331</v>
+        <v>0.001217400296474966</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -952,16 +952,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>3064</v>
+        <v>3047.4</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>0.03463617967285389</v>
+        <v>0.0331494547762802</v>
       </c>
       <c r="E34">
-        <v>0.002913837337557551</v>
+        <v>0.002788763655782303</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -969,16 +969,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>3081.813926466619</v>
+        <v>3064.813926466619</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>0.01025786663621027</v>
+        <v>0.009817557518465999</v>
       </c>
       <c r="E35">
-        <v>0.001599344798118806</v>
+        <v>0.001530694451803839</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -986,16 +986,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>3096.712914411186</v>
+        <v>3078.112914411186</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36">
-        <v>0.007476346500770412</v>
+        <v>0.01021414327095403</v>
       </c>
       <c r="E36">
-        <v>0.001027284252014255</v>
+        <v>0.0007919514663363961</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1003,16 +1003,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>3133.618862442509</v>
+        <v>3119.418862442509</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>0.01237648045970882</v>
+        <v>0.01184523186921175</v>
       </c>
       <c r="E37">
-        <v>0.00161674744743944</v>
+        <v>0.001547350109041175</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1020,16 +1020,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>3155.20165968082</v>
+        <v>3140.60165968082</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>0.003973759564147854</v>
+        <v>0.003803189734194964</v>
       </c>
       <c r="E38">
-        <v>0.002406643116314897</v>
+        <v>0.002303340261554697</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1037,16 +1037,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>3168.125784376794</v>
+        <v>3154.525784376794</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39">
-        <v>0.00385444869379247</v>
+        <v>0.001945554753831514</v>
       </c>
       <c r="E39">
-        <v>0.0009496467796300289</v>
+        <v>0.0004793395770309529</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1054,16 +1054,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>3180.855405406395</v>
+        <v>3171.655405406395</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40">
-        <v>0.008892275482153213</v>
+        <v>0.003706166898006592</v>
       </c>
       <c r="E40">
-        <v>0.000994530810504012</v>
+        <v>0.0005053863951827171</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1071,16 +1071,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>3192.810075633211</v>
+        <v>3181.210075633211</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>0.02308051077533096</v>
+        <v>0.02208980191773095</v>
       </c>
       <c r="E41">
-        <v>0.002778734712509133</v>
+        <v>0.002659460181741564</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1088,16 +1088,16 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>3224.072026396334</v>
+        <v>3212.072026396334</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42">
-        <v>0.003778260321143645</v>
+        <v>0.002027262432905774</v>
       </c>
       <c r="E42">
-        <v>0.001104414555411244</v>
+        <v>0.0004721022104027146</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1105,16 +1105,16 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>3243.873355870091</v>
+        <v>3231.273355870092</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43">
-        <v>0.002493016360014469</v>
+        <v>0.001160092827437504</v>
       </c>
       <c r="E43">
-        <v>0.0002627792643487508</v>
+        <v>0.0005248038981264897</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1122,16 +1122,16 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>3259.461277156506</v>
+        <v>3249.661277156506</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>0.003520979003111298</v>
+        <v>0.005866434030802336</v>
       </c>
       <c r="E44">
-        <v>0.001029209247063302</v>
+        <v>0.0005087181939129394</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1139,16 +1139,16 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>3275.706563811741</v>
+        <v>3264.906563811741</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>0.006690400924903099</v>
+        <v>0.006587785431038932</v>
       </c>
       <c r="E45">
-        <v>0.0004779330702489417</v>
+        <v>0.0004706482710866217</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1156,16 +1156,16 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>3297.170677130526</v>
+        <v>3286.170677130526</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
       <c r="D46">
-        <v>0.007114685598151072</v>
+        <v>0.01082012791090631</v>
       </c>
       <c r="E46">
-        <v>0.0008559020268452416</v>
+        <v>0.0006869922483115117</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1173,16 +1173,16 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>3322.739257221812</v>
+        <v>3310.539257221813</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>0.004031759145448133</v>
+        <v>0.003987701300459387</v>
       </c>
       <c r="E47">
-        <v>0.000309780126409277</v>
+        <v>0.0003063996735747506</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1190,16 +1190,16 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>3340.274605893867</v>
+        <v>3327.874605893868</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>0.008720165543479061</v>
+        <v>0.01318027027306804</v>
       </c>
       <c r="E48">
-        <v>0.000382519680734768</v>
+        <v>0.001289983899066233</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1207,16 +1207,16 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>3363.00085761773</v>
+        <v>3350.20085761773</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>0.01098980593122331</v>
+        <v>0.01085366562236222</v>
       </c>
       <c r="E49">
-        <v>0.000464825000048043</v>
+        <v>0.0004585738651058436</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1224,16 +1224,16 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>3380.649591047521</v>
+        <v>3368.24959104752</v>
       </c>
       <c r="C50">
         <v>3</v>
       </c>
       <c r="D50">
-        <v>0.007028112719978081</v>
+        <v>0.01357043037958504</v>
       </c>
       <c r="E50">
-        <v>0.001509742732439736</v>
+        <v>0.0009480711635052563</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1241,16 +1241,16 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>3395.65849793409</v>
+        <v>3383.85849793409</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>0.006788603562007698</v>
+        <v>0.006684249939476672</v>
       </c>
       <c r="E51">
-        <v>0.0005157876535650174</v>
+        <v>0.0005088623488223971</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1258,16 +1258,16 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>3411.582461109694</v>
+        <v>3401.382461109694</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>0.01316921060467234</v>
+        <v>0.0130655937434392</v>
       </c>
       <c r="E52">
-        <v>0.0004666798297619102</v>
+        <v>0.0004628791821704674</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1275,16 +1275,16 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>3430.405841076768</v>
+        <v>3420.405841076768</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>0.008655787788784879</v>
+        <v>0.008576425709640234</v>
       </c>
       <c r="E53">
-        <v>0.0003797168811668873</v>
+        <v>0.0003760143836651919</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1292,16 +1292,16 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>3452.040838634491</v>
+        <v>3441.040838634491</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>0.006101726008472538</v>
+        <v>0.02324036883432738</v>
       </c>
       <c r="E54">
-        <v>0.0009152589012708806</v>
+        <v>0.00185922950674619</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1309,16 +1309,16 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>3477.521886486277</v>
+        <v>3466.321886486277</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>0.006343840521350375</v>
+        <v>0.006071537232359859</v>
       </c>
       <c r="E55">
-        <v>0.001585960130337594</v>
+        <v>0.001517884308089965</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1326,16 +1326,16 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>3485.001985506649</v>
+        <v>3474.201985506649</v>
       </c>
       <c r="C56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D56">
-        <v>0.006843909527091864</v>
+        <v>0.003528602170120224</v>
       </c>
       <c r="E56">
-        <v>0.0009058115550562761</v>
+        <v>0.0004670208754570885</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1343,16 +1343,16 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>3503.741363695906</v>
+        <v>3493.141363695906</v>
       </c>
       <c r="C57">
         <v>3</v>
       </c>
       <c r="D57">
-        <v>0.01364478371902552</v>
+        <v>0.02019293873546069</v>
       </c>
       <c r="E57">
-        <v>0.001049598747617347</v>
+        <v>0.001429588583041465</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1360,16 +1360,16 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>3521.461101658533</v>
+        <v>3510.661101658533</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D58">
-        <v>0.005134959864739125</v>
+        <v>0.008325312827123963</v>
       </c>
       <c r="E58">
-        <v>0.0006544222277116336</v>
+        <v>0.001800986040153347</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1377,16 +1377,16 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>3536.043535477975</v>
+        <v>3525.443535477975</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>0.00612602588370704</v>
+        <v>0.005863072079783329</v>
       </c>
       <c r="E59">
-        <v>0.00637606775651141</v>
+        <v>0.006102381144264281</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1394,16 +1394,16 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>3545.218978961481</v>
+        <v>3536.818978961481</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
-        <v>0.04215767530712843</v>
+        <v>0.01894605808449602</v>
       </c>
       <c r="E60">
-        <v>0.00664987140261252</v>
+        <v>0.000777084289884611</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1411,16 +1411,16 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>3561.667933967139</v>
+        <v>3553.059086400061</v>
       </c>
       <c r="C61">
         <v>3</v>
       </c>
       <c r="D61">
-        <v>0.007645409937961853</v>
+        <v>0.009414025475432353</v>
       </c>
       <c r="E61">
-        <v>0.001078198837404877</v>
+        <v>0.0008765386848633476</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1428,16 +1428,16 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>3580.019183465469</v>
+        <v>3572.945718819506</v>
       </c>
       <c r="C62">
         <v>3</v>
       </c>
       <c r="D62">
-        <v>0.008299175502610256</v>
+        <v>0.008934202554999708</v>
       </c>
       <c r="E62">
-        <v>0.0006840855412917909</v>
+        <v>0.0009266394039432185</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1445,16 +1445,16 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>3589.932337372161</v>
+        <v>3581.276241950112</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>0.03162934850620898</v>
+        <v>0.03027168896261209</v>
       </c>
       <c r="E63">
-        <v>0.002231909672817166</v>
+        <v>0.002136107084055289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sucessfully extracted occupancies for 116Cd
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_3_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_3_spec_factors.xlsx
@@ -428,13 +428,13 @@
         <v>2205</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.02911706285278049</v>
+        <v>0.03807553614380086</v>
       </c>
       <c r="E3">
-        <v>0.0007742253544701382</v>
+        <v>0.001649131501769719</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -445,13 +445,13 @@
         <v>2232</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.08259227143154145</v>
+        <v>0.07421083397630317</v>
       </c>
       <c r="E4">
-        <v>0.001848109445836572</v>
+        <v>0.002087028032034687</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2470.366758096668</v>
+        <v>2470.566758096668</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2481.984729487203</v>
+        <v>2482.584729487203</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -496,13 +496,13 @@
         <v>2497.913976174627</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0.003373297067722395</v>
+        <v>0.01812079843763099</v>
       </c>
       <c r="E7">
-        <v>0.0008187614242044651</v>
+        <v>0.0007123348598917967</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -516,10 +516,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.01728622194449643</v>
+        <v>0.01719593543409337</v>
       </c>
       <c r="E8">
-        <v>0.0006630908488656306</v>
+        <v>0.0006516127066592582</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -530,13 +530,13 @@
         <v>2593.831325411606</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>0.02208428679384985</v>
+        <v>0.01169292715860255</v>
       </c>
       <c r="E9">
-        <v>0.001495566083159258</v>
+        <v>0.001148203268079208</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -550,10 +550,10 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0.0268483955912421</v>
+        <v>0.02626145343863209</v>
       </c>
       <c r="E10">
-        <v>0.001054856487612694</v>
+        <v>0.001020999307578782</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -564,13 +564,13 @@
         <v>2621.783451658836</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>0.00309447226499785</v>
+        <v>0.003022396703061827</v>
       </c>
       <c r="E11">
-        <v>0.0006268501198112199</v>
+        <v>0.0009764666271430518</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -584,10 +584,10 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0.01149130537220409</v>
+        <v>0.01093761998669994</v>
       </c>
       <c r="E12">
-        <v>0.0006675264545959958</v>
+        <v>0.0006440978654129237</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -598,13 +598,13 @@
         <v>2649.075587546623</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>0.01472230434964875</v>
+        <v>0.01543155789994548</v>
       </c>
       <c r="E13">
-        <v>0.0007573561146787284</v>
+        <v>0.001178157863618592</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -615,13 +615,13 @@
         <v>2664.601302816965</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.007289291180016085</v>
+        <v>0.008538734288540894</v>
       </c>
       <c r="E14">
-        <v>0.0006598198330066742</v>
+        <v>0.0009896646210438237</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -635,10 +635,10 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0.01800662804138555</v>
+        <v>0.01785136717517294</v>
       </c>
       <c r="E15">
-        <v>0.000931406133057303</v>
+        <v>0.0009051469308598815</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -649,13 +649,13 @@
         <v>2702.26533490114</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>0.004391319269637482</v>
+        <v>0.04060174722303102</v>
       </c>
       <c r="E16">
-        <v>0.0007582133990740976</v>
+        <v>0.001615856980916849</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -666,13 +666,13 @@
         <v>2715.640802344541</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>0.0104679443723541</v>
+        <v>0.01159582284168615</v>
       </c>
       <c r="E17">
-        <v>0.0005962120273638413</v>
+        <v>0.0008606274765313941</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -686,10 +686,10 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>0.02780269134025979</v>
+        <v>0.02665576337872482</v>
       </c>
       <c r="E18">
-        <v>0.00110310367550748</v>
+        <v>0.001064855733249467</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -697,16 +697,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2749.680085527932</v>
+        <v>2749.880085527932</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>0.01406444463080108</v>
+        <v>0.01449933027765855</v>
       </c>
       <c r="E19">
-        <v>0.001024149975157255</v>
+        <v>0.001616024427231293</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -734,13 +734,13 @@
         <v>2779.2</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0.07348957557846092</v>
+        <v>0.04851787932698472</v>
       </c>
       <c r="E21">
-        <v>0.002774143209893858</v>
+        <v>0.00121145340602076</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -768,13 +768,13 @@
         <v>2828.359721907576</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>0.002374588601064437</v>
+        <v>0.001325443346966772</v>
       </c>
       <c r="E23">
-        <v>0.000315379793147412</v>
+        <v>0.0001743078728063171</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -887,13 +887,13 @@
         <v>2949.317122042539</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>0.04751149746237109</v>
+        <v>0.0295946834879278</v>
       </c>
       <c r="E30">
-        <v>0.001910788484899707</v>
+        <v>0.0007853605849685846</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -938,13 +938,13 @@
         <v>2997.718657087334</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>0.01747133954907086</v>
+        <v>0.004259860495121163</v>
       </c>
       <c r="E33">
-        <v>0.001217400296474966</v>
+        <v>0.001419953498373721</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -955,13 +955,13 @@
         <v>3047.4</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>0.0331494547762802</v>
+        <v>0.02124980265850609</v>
       </c>
       <c r="E34">
-        <v>0.002788763655782303</v>
+        <v>0.0008424112900538539</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1006,13 +1006,13 @@
         <v>3119.418862442509</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>0.01184523186921175</v>
+        <v>0.005900999224678612</v>
       </c>
       <c r="E37">
-        <v>0.001547350109041175</v>
+        <v>0.0005619999261598677</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1043,10 +1043,10 @@
         <v>2</v>
       </c>
       <c r="D39">
-        <v>0.001945554753831514</v>
+        <v>0.004701757321759495</v>
       </c>
       <c r="E39">
-        <v>0.0004793395770309529</v>
+        <v>0.001158403977824803</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1057,13 +1057,13 @@
         <v>3171.655405406395</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <v>0.003706166898006592</v>
+        <v>0.006531558847255968</v>
       </c>
       <c r="E40">
-        <v>0.0005053863951827171</v>
+        <v>0.00340432764160008</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1094,10 +1094,10 @@
         <v>2</v>
       </c>
       <c r="D42">
-        <v>0.002027262432905774</v>
+        <v>0.004899217546188956</v>
       </c>
       <c r="E42">
-        <v>0.0004721022104027146</v>
+        <v>0.001140913675139894</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1111,10 +1111,10 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <v>0.001160092827437504</v>
+        <v>0.002803557666307301</v>
       </c>
       <c r="E43">
-        <v>0.0005248038981264897</v>
+        <v>0.001268276087139017</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1125,13 +1125,13 @@
         <v>3249.661277156506</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>0.005866434030802336</v>
+        <v>0.005948902094598789</v>
       </c>
       <c r="E44">
-        <v>0.0005087181939129394</v>
+        <v>0.0006953262188492091</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1142,13 +1142,13 @@
         <v>3264.906563811741</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D45">
-        <v>0.006587785431038932</v>
+        <v>0.007395361199218036</v>
       </c>
       <c r="E45">
-        <v>0.0004706482710866217</v>
+        <v>0.0006530968331776967</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1210,13 +1210,13 @@
         <v>3350.20085761773</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D49">
-        <v>0.01085366562236222</v>
+        <v>0.0112606585593418</v>
       </c>
       <c r="E49">
-        <v>0.0004585738651058436</v>
+        <v>0.0007295111026816115</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1247,10 +1247,10 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>0.006684249939476672</v>
+        <v>0.006682619188758948</v>
       </c>
       <c r="E51">
-        <v>0.0005088623488223971</v>
+        <v>0.000506707252974176</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1264,10 +1264,10 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>0.0130655937434392</v>
+        <v>0.0130488628990849</v>
       </c>
       <c r="E52">
-        <v>0.0004628791821704674</v>
+        <v>0.0004610066028577759</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1281,10 +1281,10 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>0.008576425709640234</v>
+        <v>0.008578015564787749</v>
       </c>
       <c r="E53">
-        <v>0.0003760143836651919</v>
+        <v>0.0003750479024411025</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1329,13 +1329,13 @@
         <v>3474.201985506649</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>0.003528602170120224</v>
+        <v>0.02454167604123628</v>
       </c>
       <c r="E56">
-        <v>0.0004670208754570885</v>
+        <v>0.001761364309179637</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1346,13 +1346,13 @@
         <v>3493.141363695906</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <v>0.02019293873546069</v>
+        <v>0.02308149543432147</v>
       </c>
       <c r="E57">
-        <v>0.001429588583041465</v>
+        <v>0.0007372586188144812</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1363,13 +1363,13 @@
         <v>3510.661101658533</v>
       </c>
       <c r="C58">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>0.008325312827123963</v>
+        <v>0.008149115499999781</v>
       </c>
       <c r="E58">
-        <v>0.001800986040153347</v>
+        <v>0.00184396044160579</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1400,10 +1400,10 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <v>0.01894605808449602</v>
+        <v>0.01910140741942075</v>
       </c>
       <c r="E60">
-        <v>0.000777084289884611</v>
+        <v>0.000745097717852869</v>
       </c>
     </row>
     <row r="61" spans="1:5">

</xml_diff>